<commit_message>
completed optimization diagnostics tests
</commit_message>
<xml_diff>
--- a/test-files/additional-sheet-test-files/optimization-diagnostics-unknown-parameter.xlsx
+++ b/test-files/additional-sheet-test-files/optimization-diagnostics-unknown-parameter.xlsx
@@ -9051,7 +9051,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L22" activeCellId="0" sqref="L22"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9102,6 +9102,9 @@
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>53</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>0.2342</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>